<commit_message>
update template peserta dan rab
</commit_message>
<xml_diff>
--- a/public/referensi/template upload Peserta dan RAB.xlsx
+++ b/public/referensi/template upload Peserta dan RAB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\application_letters\public\referensi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C43093-591F-4508-8331-D6E1D08847DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3020C397-8907-4B8C-ACC5-DDDAA6E0E6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6CA4C54B-CC02-43B2-9E43-2B376088AE04}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="9420" xr2:uid="{6CA4C54B-CC02-43B2-9E43-2B376088AE04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Pilih Narasumber dan Moderator</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Penanggung Jawab</t>
-  </si>
-  <si>
-    <t>Ketua</t>
   </si>
   <si>
     <t>Bambang</t>
@@ -242,6 +239,36 @@
   <si>
     <t xml:space="preserve">  Pangkat (Golongan) </t>
   </si>
+  <si>
+    <t>Ketua Panitia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pastikan peran kepanitiaan sebagai "Ketua Panitia" ada didalam tabel agar sistem dapat mengidentifikasi panitia penandatangan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -253,7 +280,7 @@
     <numFmt numFmtId="166" formatCode="[$Rp-421]#,##0"/>
     <numFmt numFmtId="167" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +317,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -322,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,6 +377,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,7 +793,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +813,7 @@
     <col min="13" max="13" width="26.5546875" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.88671875" customWidth="1"/>
+    <col min="16" max="16" width="59.109375" customWidth="1"/>
     <col min="17" max="17" width="9.5546875" customWidth="1"/>
     <col min="18" max="18" width="5.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.21875" style="4" bestFit="1" customWidth="1"/>
@@ -811,7 +855,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S1" s="8"/>
       <c r="T1" s="8"/>
@@ -820,7 +864,7 @@
       <c r="W1" s="8"/>
       <c r="X1" s="2"/>
       <c r="Z1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="8"/>
       <c r="AB1" s="8"/>
@@ -835,16 +879,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -856,34 +900,37 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L2" t="s">
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" t="s">
         <v>49</v>
       </c>
-      <c r="N2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" t="s">
-        <v>50</v>
+      <c r="P2" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="R2" t="s">
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" t="s">
         <v>49</v>
-      </c>
-      <c r="U2" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" t="s">
-        <v>50</v>
       </c>
       <c r="W2" t="s">
         <v>3</v>
@@ -892,25 +939,25 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" t="s">
-        <v>42</v>
-      </c>
       <c r="AC2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>30</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -921,13 +968,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>54</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -945,32 +992,35 @@
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O3" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>57</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X3" s="6"/>
       <c r="Z3">
         <v>1</v>
       </c>
       <c r="AA3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB3" t="s">
         <v>32</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -990,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
@@ -999,10 +1049,10 @@
         <v>2</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X4" s="6"/>
       <c r="Z4">
@@ -1012,16 +1062,16 @@
         <v>525112</v>
       </c>
       <c r="AB4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC4" t="s">
         <v>34</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>35</v>
       </c>
       <c r="AD4">
         <v>170</v>
       </c>
       <c r="AE4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AF4" s="5">
         <v>30000</v>
@@ -1036,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -1048,19 +1098,19 @@
         <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R5">
         <v>3</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X5" s="6"/>
       <c r="Z5">
@@ -1070,16 +1120,16 @@
         <v>525112</v>
       </c>
       <c r="AB5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AD5">
         <v>170</v>
       </c>
       <c r="AE5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AF5" s="5">
         <v>15000</v>
@@ -1091,10 +1141,10 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
         <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -1103,17 +1153,17 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R6">
         <v>4</v>
       </c>
       <c r="S6" s="1"/>
       <c r="W6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X6" s="6"/>
       <c r="Z6">
@@ -1123,16 +1173,16 @@
         <v>525113</v>
       </c>
       <c r="AB6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC6" t="s">
         <v>37</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>38</v>
       </c>
       <c r="AD6">
         <v>3</v>
       </c>
       <c r="AE6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AF6" s="5">
         <v>900000</v>
@@ -1147,19 +1197,19 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R7">
         <v>5</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X7" s="6"/>
       <c r="Z7">
@@ -1171,37 +1221,37 @@
         <v>6</v>
       </c>
       <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
         <v>17</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
       </c>
       <c r="R8">
         <v>6</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X8" s="6"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="K9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R9">
         <v>7</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W9" t="s">
         <v>47</v>
-      </c>
-      <c r="W9" t="s">
-        <v>48</v>
       </c>
       <c r="X9" s="6"/>
     </row>

</xml_diff>

<commit_message>
ubah redaksi ketua panitia jadi ketua
</commit_message>
<xml_diff>
--- a/public/referensi/template upload Peserta dan RAB.xlsx
+++ b/public/referensi/template upload Peserta dan RAB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\application_letters\public\referensi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3020C397-8907-4B8C-ACC5-DDDAA6E0E6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F284A302-D24B-4651-BFBD-4B854EED4CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="9420" xr2:uid="{6CA4C54B-CC02-43B2-9E43-2B376088AE04}"/>
   </bookViews>
@@ -240,12 +240,6 @@
     <t xml:space="preserve">  Pangkat (Golongan) </t>
   </si>
   <si>
-    <t>Ketua Panitia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pastikan peran kepanitiaan sebagai "Ketua Panitia" ada didalam tabel agar sistem dapat mengidentifikasi panitia penandatangan</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -268,6 +262,12 @@
       </rPr>
       <t>Note:</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pastikan peran kepanitiaan sebagai "Ketua" ada didalam tabel agar sistem dapat mengidentifikasi panitia penandatangan</t>
+  </si>
+  <si>
+    <t>Ketua</t>
   </si>
 </sst>
 </file>
@@ -374,10 +374,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59B9331-4B57-4138-BDB9-703DEB8172AA}">
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,46 +833,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
       <c r="X1" s="2"/>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -914,8 +914,8 @@
       <c r="O2" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>58</v>
+      <c r="P2" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="R2" t="s">
         <v>1</v>
@@ -1040,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>

</xml_diff>